<commit_message>
Updated something in the BetII.xlsx
</commit_message>
<xml_diff>
--- a/ANI/BetII.xlsx
+++ b/ANI/BetII.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8360" yWindow="500" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="18760" yWindow="7100" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ANI" sheetId="1" r:id="rId1"/>
@@ -596,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA24" sqref="AA24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4583,7 +4583,7 @@
   <dimension ref="A1:AJ36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>